<commit_message>
Fix Adicionar custo ao GridySearch
</commit_message>
<xml_diff>
--- a/A_STAR_Results.xlsx
+++ b/A_STAR_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno Oliveira\Desktop\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86755A95-8003-453A-B852-61D36326F383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D20B9-18C6-45A8-8F96-ABB9833AFB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>File Path</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Execution Time Product to Output</t>
+  </si>
+  <si>
+    <t>./Matriz_Random\MatrizRandom.txt</t>
   </si>
   <si>
     <t>./Matriz_Random\Matriz10x10\HighDensity\MatrizRandom_10x10_HighDensity_1.txt</t>
@@ -610,11 +613,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -647,16 +648,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>2.9733180999755859E-3</v>
+        <v>3.4113168716430657E-2</v>
       </c>
       <c r="E2">
-        <v>2.0022392272949219E-3</v>
+        <v>1.029014587402344E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -664,16 +665,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>2.3407936096191411E-3</v>
+        <v>2.0017623901367192E-3</v>
       </c>
       <c r="E3">
-        <v>2.746820449829102E-3</v>
+        <v>1.0132789611816411E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,16 +682,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>1.4855861663818359E-3</v>
+        <v>1.9845962524414058E-3</v>
       </c>
       <c r="E4">
-        <v>4.0860176086425781E-3</v>
+        <v>1.998662948608398E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -698,16 +699,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D5">
-        <v>9.1552734375E-4</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1.9984245300292969E-3</v>
+        <v>2.0000934600830078E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -715,16 +716,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>4.0025711059570313E-3</v>
+        <v>9.9968910217285156E-4</v>
       </c>
       <c r="E6">
-        <v>9.9873542785644531E-4</v>
+        <v>1.998662948608398E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,16 +733,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>1.9998550415039058E-3</v>
+        <v>1.998662948608398E-3</v>
       </c>
       <c r="E7">
-        <v>9.9897384643554688E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,16 +750,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>2.0020008087158199E-3</v>
+        <v>3.0016899108886719E-3</v>
       </c>
       <c r="E8">
-        <v>5.0015449523925781E-3</v>
+        <v>9.9921226501464844E-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,16 +767,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>2.0012855529785161E-3</v>
+        <v>1.000404357910156E-3</v>
       </c>
       <c r="E9">
-        <v>9.8180770874023438E-4</v>
+        <v>6.9801807403564453E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -783,16 +784,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10">
-        <v>2.0003318786621089E-3</v>
+        <v>3.0004978179931641E-3</v>
       </c>
       <c r="E10">
-        <v>9.9945068359375E-4</v>
+        <v>2.0020008087158199E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -803,13 +804,13 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>1.9993782043457031E-3</v>
+        <v>2.0005702972412109E-3</v>
       </c>
       <c r="E11">
-        <v>1.0583400726318359E-3</v>
+        <v>9.9968910217285156E-4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -817,16 +818,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>9.8824501037597656E-4</v>
+        <v>1.9993782043457031E-3</v>
       </c>
       <c r="E12">
-        <v>2.9845237731933589E-3</v>
+        <v>9.9921226501464844E-4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -834,16 +835,16 @@
         <v>16</v>
       </c>
       <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
         <v>17</v>
       </c>
-      <c r="C13">
-        <v>19</v>
-      </c>
       <c r="D13">
-        <v>2.0031929016113281E-3</v>
+        <v>1.2152194976806641E-3</v>
       </c>
       <c r="E13">
-        <v>2.0008087158203121E-3</v>
+        <v>2.807378768920898E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,16 +852,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D14">
-        <v>9.9897384643554688E-4</v>
+        <v>9.9992752075195313E-4</v>
       </c>
       <c r="E14">
-        <v>1.002311706542969E-3</v>
+        <v>2.99835205078125E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,16 +869,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D15">
-        <v>9.9802017211914063E-4</v>
+        <v>1.0001659393310549E-3</v>
       </c>
       <c r="E15">
-        <v>4.0199756622314453E-3</v>
+        <v>1.0008811950683589E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,16 +886,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D16">
-        <v>7.0154666900634774E-3</v>
+        <v>9.9873542785644531E-4</v>
       </c>
       <c r="E16">
-        <v>1.5985965728759769E-2</v>
+        <v>4.0006637573242188E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,13 +906,13 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D17">
-        <v>2.0322799682617192E-3</v>
+        <v>6.0014724731445313E-3</v>
       </c>
       <c r="E17">
-        <v>1.99122428894043E-2</v>
+        <v>1.6005277633666989E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -919,16 +920,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C18">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D18">
-        <v>2.0008087158203121E-3</v>
+        <v>2.0346641540527339E-3</v>
       </c>
       <c r="E18">
-        <v>1.9954681396484378E-2</v>
+        <v>2.0997762680053711E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -936,16 +937,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="D19">
-        <v>1.800179481506348E-2</v>
+        <v>2.0022392272949219E-3</v>
       </c>
       <c r="E19">
-        <v>1.9972324371337891E-3</v>
+        <v>2.1092414855957031E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -953,16 +954,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D20">
-        <v>6.1344146728515618E-2</v>
+        <v>1.8035173416137699E-2</v>
       </c>
       <c r="E20">
-        <v>9.9992752075195313E-4</v>
+        <v>2.2675991058349609E-3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -970,16 +971,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>3.1000137329101559E-2</v>
+        <v>6.599736213684082E-2</v>
       </c>
       <c r="E21">
-        <v>1.9977092742919922E-3</v>
+        <v>1.2340545654296879E-3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -987,16 +988,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D22">
-        <v>3.5042762756347663E-2</v>
+        <v>3.1324148178100593E-2</v>
       </c>
       <c r="E22">
-        <v>2.0339488983154301E-3</v>
+        <v>1.5647411346435549E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,16 +1005,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C23">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D23">
-        <v>4.5347213745117188E-4</v>
+        <v>3.6482810974121087E-2</v>
       </c>
       <c r="E23">
-        <v>5.5001735687255859E-2</v>
+        <v>3.0193328857421879E-3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,16 +1022,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D24">
-        <v>6.5629005432128906E-2</v>
+        <v>2.0384788513183589E-3</v>
       </c>
       <c r="E24">
-        <v>3.0565261840820308E-3</v>
+        <v>5.5961132049560547E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,16 +1039,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D25">
-        <v>3.2091856002807617E-2</v>
+        <v>6.8179130554199219E-2</v>
       </c>
       <c r="E25">
-        <v>1.9984245300292969E-3</v>
+        <v>3.0336380004882808E-3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,16 +1056,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>6.9985389709472656E-3</v>
+        <v>3.4812688827514648E-2</v>
       </c>
       <c r="E26">
-        <v>3.0002593994140621E-3</v>
+        <v>2.0270347595214839E-3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,16 +1073,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D27">
-        <v>4.4495105743408203E-2</v>
+        <v>7.9710483551025391E-3</v>
       </c>
       <c r="E27">
-        <v>1.0895729064941411E-3</v>
+        <v>2.0077228546142578E-3</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,16 +1090,16 @@
         <v>31</v>
       </c>
       <c r="B28">
+        <v>50</v>
+      </c>
+      <c r="C28">
         <v>10</v>
       </c>
-      <c r="C28">
-        <v>52</v>
-      </c>
       <c r="D28">
-        <v>9.9611282348632813E-4</v>
+        <v>4.5490264892578118E-2</v>
       </c>
       <c r="E28">
-        <v>5.8111906051635742E-2</v>
+        <v>1.0087490081787109E-3</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,16 +1107,16 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D29">
-        <v>4.9083232879638672E-3</v>
+        <v>2.056360244750977E-3</v>
       </c>
       <c r="E29">
-        <v>8.0003738403320313E-3</v>
+        <v>5.7945013046264648E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,16 +1124,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C30">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="D30">
-        <v>1.9650459289550781E-3</v>
+        <v>4.7783851623535156E-3</v>
       </c>
       <c r="E30">
-        <v>0.15765190124511719</v>
+        <v>7.9977512359619141E-3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,16 +1141,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>155</v>
+        <v>35</v>
       </c>
       <c r="C31">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D31">
-        <v>8.0921173095703125E-2</v>
+        <v>2.998590469360352E-3</v>
       </c>
       <c r="E31">
-        <v>1.8946170806884769E-2</v>
+        <v>0.16624116897583011</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1157,16 +1158,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>56</v>
+        <v>155</v>
       </c>
       <c r="C32">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D32">
-        <v>8.0010890960693359E-3</v>
+        <v>8.285975456237793E-2</v>
       </c>
       <c r="E32">
-        <v>6.2076330184936523E-2</v>
+        <v>2.1047592163085941E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,16 +1175,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="C33">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="D33">
-        <v>6.5104246139526367E-2</v>
+        <v>8.0020427703857422E-3</v>
       </c>
       <c r="E33">
-        <v>1.4009952545166021E-2</v>
+        <v>6.3354969024658203E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1191,16 +1192,16 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="C34">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="D34">
-        <v>1.099705696105957E-2</v>
+        <v>7.0831537246704102E-2</v>
       </c>
       <c r="E34">
-        <v>9.0010881423950195E-2</v>
+        <v>1.5001773834228521E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,16 +1209,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C35">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="D35">
-        <v>5.7996273040771477E-2</v>
+        <v>1.10013484954834E-2</v>
       </c>
       <c r="E35">
-        <v>4.3927192687988281E-2</v>
+        <v>9.4768047332763672E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,16 +1226,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C36">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D36">
-        <v>0.2140498161315918</v>
+        <v>6.1228752136230469E-2</v>
       </c>
       <c r="E36">
-        <v>1.7915248870849609E-2</v>
+        <v>4.5001506805419922E-2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,16 +1243,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C37">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D37">
-        <v>9.8056316375732422E-2</v>
+        <v>0.22191691398620611</v>
       </c>
       <c r="E37">
-        <v>6.3998937606811523E-2</v>
+        <v>1.8947124481201168E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,16 +1260,16 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="C38">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D38">
-        <v>4.9989223480224609E-3</v>
+        <v>0.1000323295593262</v>
       </c>
       <c r="E38">
-        <v>0.29902386665344238</v>
+        <v>6.5999984741210938E-2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,16 +1277,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="C39">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="D39">
-        <v>8.1138849258422852E-2</v>
+        <v>5.0134658813476563E-3</v>
       </c>
       <c r="E39">
-        <v>2.30555534362793E-2</v>
+        <v>0.31123852729797358</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,16 +1294,16 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C40">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="D40">
-        <v>2.0002365112304691E-2</v>
+        <v>7.7059030532836914E-2</v>
       </c>
       <c r="E40">
-        <v>4.4999599456787109E-2</v>
+        <v>2.3279905319213871E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,16 +1311,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C41">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="D41">
-        <v>4.9657821655273438E-3</v>
+        <v>2.1000862121582031E-2</v>
       </c>
       <c r="E41">
-        <v>0.23817682266235349</v>
+        <v>4.5008659362792969E-2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,16 +1328,16 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="C42">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="D42">
-        <v>0.31999325752258301</v>
+        <v>5.9747695922851563E-3</v>
       </c>
       <c r="E42">
-        <v>3.0000209808349609E-3</v>
+        <v>0.24637413024902341</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,16 +1345,16 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D43">
-        <v>0.29751324653625488</v>
+        <v>0.34087944030761719</v>
       </c>
       <c r="E43">
-        <v>1.0008811950683589E-3</v>
+        <v>3.4022331237792969E-3</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,16 +1362,16 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="C44">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D44">
-        <v>7.9002141952514648E-2</v>
+        <v>0.32491922378540039</v>
       </c>
       <c r="E44">
-        <v>1.8229007720947269E-2</v>
+        <v>2.006769180297852E-3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,16 +1379,16 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="C45">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D45">
-        <v>8.5446834564208984E-2</v>
+        <v>8.0690383911132813E-2</v>
       </c>
       <c r="E45">
-        <v>4.0555000305175781E-3</v>
+        <v>1.900792121887207E-2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,16 +1396,16 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="C46">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="D46">
-        <v>2.3087978363037109E-2</v>
+        <v>8.8779211044311523E-2</v>
       </c>
       <c r="E46">
-        <v>7.7110767364501953E-2</v>
+        <v>3.1838417053222661E-3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,16 +1413,16 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C47">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D47">
-        <v>2.9747486114501949E-3</v>
+        <v>2.457427978515625E-2</v>
       </c>
       <c r="E47">
-        <v>0.12806010246276861</v>
+        <v>8.5585117340087891E-2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,16 +1430,16 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C48">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="D48">
-        <v>2.9124021530151371E-2</v>
+        <v>2.9735565185546879E-3</v>
       </c>
       <c r="E48">
-        <v>2.49481201171875E-2</v>
+        <v>0.1296195983886719</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,16 +1447,16 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="C49">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D49">
-        <v>9.0012550354003906E-3</v>
+        <v>3.0000209808349609E-2</v>
       </c>
       <c r="E49">
-        <v>7.0999383926391602E-2</v>
+        <v>2.7997255325317379E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,16 +1464,16 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C50">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="D50">
-        <v>0.213062047958374</v>
+        <v>8.9974403381347656E-3</v>
       </c>
       <c r="E50">
-        <v>5.0272226333618157E-2</v>
+        <v>7.6563835144042969E-2</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,16 +1481,16 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C51">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D51">
-        <v>3.4028530120849609E-2</v>
+        <v>0.25182294845581049</v>
       </c>
       <c r="E51">
-        <v>0.17207884788513181</v>
+        <v>4.9971818923950202E-2</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,16 +1498,16 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C52">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D52">
-        <v>2.9609203338623051E-3</v>
+        <v>3.6023378372192383E-2</v>
       </c>
       <c r="E52">
-        <v>0.93984246253967285</v>
+        <v>0.1826324462890625</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,16 +1515,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C53">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D53">
-        <v>1.075267791748047E-2</v>
+        <v>2.9993057250976558E-3</v>
       </c>
       <c r="E53">
-        <v>0.44551944732666021</v>
+        <v>0.9858551025390625</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,16 +1532,16 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C54">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D54">
-        <v>1.8913507461547852E-2</v>
+        <v>1.0217905044555661E-2</v>
       </c>
       <c r="E54">
-        <v>0.183643102645874</v>
+        <v>0.47397851943969732</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,16 +1549,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="C55">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D55">
-        <v>0.1320757865905762</v>
+        <v>1.9154071807861332E-2</v>
       </c>
       <c r="E55">
-        <v>3.2775402069091797E-2</v>
+        <v>0.19222903251647949</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1568,13 +1569,13 @@
         <v>79</v>
       </c>
       <c r="C56">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D56">
-        <v>0.1091017723083496</v>
+        <v>0.13407135009765619</v>
       </c>
       <c r="E56">
-        <v>4.2119979858398438E-2</v>
+        <v>3.2505512237548828E-2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,16 +1583,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C57">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D57">
-        <v>2.4000167846679691E-2</v>
+        <v>0.1121797561645508</v>
       </c>
       <c r="E57">
-        <v>9.1000080108642578E-2</v>
+        <v>4.2238473892211907E-2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,16 +1600,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="C58">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D58">
-        <v>0.33014130592346191</v>
+        <v>2.9036760330200199E-2</v>
       </c>
       <c r="E58">
-        <v>2.998590469360352E-3</v>
+        <v>0.1060874462127686</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,16 +1617,16 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="C59">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="D59">
-        <v>5.4967403411865227E-2</v>
+        <v>0.35072517395019531</v>
       </c>
       <c r="E59">
-        <v>7.6637744903564453E-2</v>
+        <v>2.5413036346435551E-3</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,16 +1634,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C60">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D60">
-        <v>2.1966457366943359E-2</v>
+        <v>5.7691574096679688E-2</v>
       </c>
       <c r="E60">
-        <v>0.36623859405517578</v>
+        <v>9.7613811492919922E-2</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,16 +1651,16 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>206</v>
+        <v>84</v>
       </c>
       <c r="C61">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="D61">
-        <v>0.4630584716796875</v>
+        <v>2.292323112487793E-2</v>
       </c>
       <c r="E61">
-        <v>3.0293464660644531E-3</v>
+        <v>0.38600897789001459</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,16 +1668,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="C62">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="D62">
-        <v>0.15818953514099121</v>
+        <v>0.48108768463134771</v>
       </c>
       <c r="E62">
-        <v>6.1278820037841797E-2</v>
+        <v>3.9598941802978524E-3</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,16 +1685,16 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="C63">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="D63">
-        <v>2.1264059543609619</v>
+        <v>0.16604042053222659</v>
       </c>
       <c r="E63">
-        <v>1.198244094848633E-2</v>
+        <v>6.3820838928222656E-2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1701,16 +1702,16 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="C64">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="D64">
-        <v>4.1005373001098633E-2</v>
+        <v>2.5724024772644039</v>
       </c>
       <c r="E64">
-        <v>1.061074495315552</v>
+        <v>1.200985908508301E-2</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1718,16 +1719,16 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C65">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D65">
-        <v>1.4002561569213871E-2</v>
+        <v>4.1589736938476563E-2</v>
       </c>
       <c r="E65">
-        <v>2.451888799667358</v>
+        <v>1.084043502807617</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1735,16 +1736,16 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C66">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="D66">
-        <v>0.46228837966918951</v>
+        <v>1.2964248657226561E-2</v>
       </c>
       <c r="E66">
-        <v>0.1038200855255127</v>
+        <v>2.581055641174316</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1752,16 +1753,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C67">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="D67">
-        <v>4.0002107620239258E-2</v>
+        <v>0.48285937309265142</v>
       </c>
       <c r="E67">
-        <v>2.1743805408477779</v>
+        <v>0.1090128421783447</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1769,16 +1770,16 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C68">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="D68">
-        <v>2.29640007019043E-2</v>
+        <v>4.2001247406005859E-2</v>
       </c>
       <c r="E68">
-        <v>1.1011366844177251</v>
+        <v>2.3508536815643311</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,16 +1787,16 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="C69">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="D69">
-        <v>0.171015739440918</v>
+        <v>2.3534297943115231E-2</v>
       </c>
       <c r="E69">
-        <v>0.25098824501037598</v>
+        <v>1.133524894714355</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1803,16 +1804,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C70">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D70">
-        <v>0.18260288238525391</v>
+        <v>0.17337131500244141</v>
       </c>
       <c r="E70">
-        <v>0.31457686424255371</v>
+        <v>0.25644946098327642</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1820,16 +1821,16 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="C71">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="D71">
-        <v>0.48578405380249018</v>
+        <v>0.1876938343048096</v>
       </c>
       <c r="E71">
-        <v>4.5017480850219727E-2</v>
+        <v>0.32822751998901373</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,16 +1838,33 @@
         <v>75</v>
       </c>
       <c r="B72">
+        <v>131</v>
+      </c>
+      <c r="C72">
+        <v>47</v>
+      </c>
+      <c r="D72">
+        <v>0.53095746040344238</v>
+      </c>
+      <c r="E72">
+        <v>4.4525384902954102E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73">
         <v>132</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>52</v>
       </c>
-      <c r="D72">
-        <v>0.79659438133239746</v>
-      </c>
-      <c r="E72">
-        <v>6.8584203720092773E-2</v>
+      <c r="D73">
+        <v>0.85325741767883301</v>
+      </c>
+      <c r="E73">
+        <v>7.200169563293457E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>